<commit_message>
Edited the CAM's class
CAM's now works for error handling staff and student :)
</commit_message>
<xml_diff>
--- a/OOPproj2002/src/pkg_camp/user_passwords.xlsx
+++ b/OOPproj2002/src/pkg_camp/user_passwords.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
   <si>
     <t>Username</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>ARVI</t>
+  </si>
+  <si>
+    <t>2cff982a584448d9b76ebaf89505905d635e000273de0313f6939f323d3575c5</t>
   </si>
 </sst>
 </file>
@@ -429,8 +432,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="13.576428571428572"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="13.576428571428572"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">

</xml_diff>